<commit_message>
add tab for text on cards for card sort tests
</commit_message>
<xml_diff>
--- a/vocabulary/SampleTypeCompilation.xlsx
+++ b/vocabulary/SampleTypeCompilation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\iSamples\metadata\vocabulary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF14527E-D75D-41A5-B20D-77DC412D3BB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46590782-9A26-45C8-8619-6C7D75E9B329}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10575" yWindow="60" windowWidth="16365" windowHeight="13605" firstSheet="2" activeTab="5" xr2:uid="{D08A62D1-934B-493D-9C48-9223CA83C33D}"/>
+    <workbookView xWindow="4680" yWindow="360" windowWidth="16455" windowHeight="13605" firstSheet="2" activeTab="5" xr2:uid="{D08A62D1-934B-493D-9C48-9223CA83C33D}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleTypes" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2076" uniqueCount="921">
   <si>
     <t>Identical split(s) of an original sample submitted blindly to the laboratory to test reproducibility (bias) of results.  Should be related to a previous original specimen.</t>
   </si>
@@ -2565,15 +2565,9 @@
     <t>[ID: 140]   [Specimen Location: Copenhagen, Zoological Museum]   [Museum Number: 205/1941]   [Period: Mesolithic]   [Date cal BC: 8550-7750]   [Date C14: 9020±280 BP]   [Taxon: Bos sp.]   [Element: mandible]   [jaw/loose: jaw]   [M3 Length (widest part): 48.5]   [M3 Width (widest part): 20.2]   [Mandible height: 69.1]   [Comments: left M3 measurements from degerbol - mandible has been stuck together]</t>
   </si>
   <si>
-    <t xml:space="preserve">[Provenience (Recorded): SC 8-12]   [Level: 90-130]   [WT (0.01 gram increments): 2.96]   [Max Size (5mm increments, maximum surficial length): 40.0]   [Class: Mammalia]   [Size 1: Medium]   [Order: Carnivora]   [Size 2: Medium]   [Family: Canidae]   [Size 3: Small]   [Genus: Lycalopex]   [Element: Humerus,  Distal &amp; Shaft]   [Comments: much bigger specimen than preceding] </t>
-  </si>
-  <si>
     <t>Specimen Type: Dental]  [Period: Pottery Neolithic]  [Taxon: Sus sp. (pig)]  [Element: dP4]  [Side: Right]  [Wear: d]</t>
   </si>
   <si>
-    <t>[Sex:   Female]  [Class:   Aves]  [Order:   Galliformes]  [Family:   Phasianidae]  [Genus:   Coturnix]  [Species:   Coturnix]  [Subspecies:   japonica]  [Common Name:   Japanese quail]  [Continent/Ocean:   North America]  [Country:   USA]  [State/Province:   MA]  [Kind2:   Skull]  [Kind4:   Complete skeleton]  [Received from:   Concord Field Station]  [Bio. Remarks:   wing chord 110, bill 11; had 3 eggs; found dead in pen]  [Site Name:   Bird Farm]  [Location:   Berlin]  [Specimen Remarks:   Complete skeleton]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[Depth (cm):  Surface]  [Condition:  Complete]  [Material Class:  Groundstone]  [Object Type:  Donut stone]  [Rock Type:  Volcanic (slightly vesicular, dacitic)]  [Weight (g):  607.9]  [Maximum Object Diameter (cm):  10.1]  [Maximum Object Thickness (cm):  5.4]  [Minimum Perforation Diameter (cm):  2.0]  [Wear Distribution:  Use-wear inside hole, most intensively at narrowest point.]  [Wear Characteristics (up To 40x):  Leveling and sheen on high areas. Most complete leveling and intense sheen at narrowest point of perforation. Rounded interstice edges and high areas.]  [Comments:  Oblong shape. Natural "fingerholds" on edges. Biconical hole. Other id# 76BW-1-8-88] </t>
   </si>
   <si>
@@ -2718,9 +2712,6 @@
     <t>buckle</t>
   </si>
   <si>
-    <t>beads</t>
-  </si>
-  <si>
     <t>block</t>
   </si>
   <si>
@@ -2790,13 +2781,205 @@
     <t>fern tissue</t>
   </si>
   <si>
-    <t>[Loc. 16]  [Laetolil Beds, Upper Unit, top part of T8]  [leaf, dicot.] Upper Pliocene [Plantae]</t>
-  </si>
-  <si>
-    <t>[Laetoli Loc 8. ]  [between tuffs 5 &amp; 7]  [seed] Pliocene  [Plantae]</t>
-  </si>
-  <si>
-    <t>[Oleisusu]  [Laetolil Beds, ?Lower Unit]  [wood] Pliocene  [Plantae]</t>
+    <t>[Material: Rock]  [Field Name: outcrop/hand specimens]  [Description: shale with a concretion]  [Collection Method: Manual]  [Geological Unit: Marcellus, facies 4, F4]  [Comment: Drawer, Cabinet 7 #4]  [Country: United States]  [State/Province: WV]  [County: Whip Gap]</t>
+  </si>
+  <si>
+    <t>shale</t>
+  </si>
+  <si>
+    <t>ooid grainstone</t>
+  </si>
+  <si>
+    <t>[Sample Name: GRF-VC]  [Other Name(s): Stratigraphic section of the LaClede Bed of the Laney Member of the Green River Formation]  [Sample Type: Terrestrial Section]  [Material: Rock]  [Classification: Sedimentary&gt;Carbonate]  [Field Name: GRF-Vermillion Creek section]  [Geological Age: Eocene]  [Latitude (WGS84): 40.773457]  [Longitude (WGS84): -108.651583]  [Locality: Vermillion Creek]  [Country: United States]  [State/Province: Colorado]  [County: Moffat]  [Collector/Chief Scientist: Elizabeth Trower]  [Collector/Chief Scientist Detail: University of Colorado Boulder]  [Collection Start Date: 2018-06-05]  [Children: {IEEJT0051 VC-18-01, IEEJT0052 VC-18-02, IEEJT0053 VC-18-03, IEEJT0054 VC-18-04, IEEJT0055 VC-18-05}]</t>
+  </si>
+  <si>
+    <t>Stratigraphic section,  LaClede Bed, Green River Formation</t>
+  </si>
+  <si>
+    <t>glass</t>
+  </si>
+  <si>
+    <t>[Sample Name: DAMA 39]  [Other Name(s): 1293]  [Sample Type: Individual Sample]  [Material: Synthetic]  [Field Name: Glass]   [Purpose: The provenance of plant ash glass in Middle East]  [Latitude (WGS84): 33.513807]  [Longitude (WGS84): 36.276528]  [Locality: Damascus]  [Country: Syria]</t>
+  </si>
+  <si>
+    <t>synthetic rock powder</t>
+  </si>
+  <si>
+    <t>[Sample Name: p4527Powder]  [Other Name(s): Min-U-Sil 40]  [Sample Type: Rock Powder]  [Material: Synthetic]</t>
+  </si>
+  <si>
+    <t>[Sample Name: Al220-5h]  [Sample Type: Experimental Specimen&gt;Other]  [Material: Synthetic]  [Field Name: Al220-5h]  [Description: Synthesized aluminum hydroxide; heated for five hours at 220 C]  [Comment: 50 mL of a 3.25 M NaOH solution were added to 30 mL of a 1.8 M Al(NO3)3 ·9H2O at a rate of 2.94 mL/min with a magnetic stirring bar for 17 minutes. The suspension was then mixed in an ultrasonic bath for 3 hours at 25˚ C, filtered, and then rinsed with nanopure water until fully desalinated. Precipitate was then heated for 5 hours at 220 C]  [Purpose: For use in Flow Adsorption Microcalorimetry research]</t>
+  </si>
+  <si>
+    <t>synthetic aluminum hydroxide</t>
+  </si>
+  <si>
+    <t>[Sample Name: 151101-NL13-WA]  [Sample Type: Individual Sample&gt;Culture]  [Material: Liquid&gt;aqueous]  [Classification: Microbiology]  [Field Name: Water]  [Collection Method: Manual]  [Size: 1 L]  [Purpose: Microbial communities analysis]  [Physiographic Feature: Channel]  [Name Of Physiographic Feature: Upper Sangamon river basin]  [Country: United States]  [State/Province: Illinois]  [County: Champaign]</t>
+  </si>
+  <si>
+    <t>water with microbial community</t>
+  </si>
+  <si>
+    <t>stream water</t>
+  </si>
+  <si>
+    <t>[Sample Name: 13626 N1-T1-1]  [Sample Type: Grab]  [Parent: IEGRL000N 13626 N1-T1-1]  [Material: Sediment]  [Field Name: bedload]  [Physiographic Feature: stream (deglaciated)]  [Name Of Physiographic Feature: Nerumaq]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Sample Name: 13626 N1-T1-1]  [Sample Type: Grab]  [Parent:  IEGRL000N 13626 N1-T1-1]  [Material: Liquid&gt;aqueous]  [Classification: Not Provided]  [Field Name: surface water]  [Physiographic Feature: stream (deglaciated)]  [Name Of Physiographic Feature: Nerumaq] </t>
+  </si>
+  <si>
+    <t>[Sample Name: ODM_DR03]  [Sample Type: Dredge]  [Description: serpentinized peridotites, hydrothermal breccias, felsic veins]  [Collection Method: dredge]  [Size: 115 kg]  [Physiographic Feature: mid-ocean ridge]  [Name Of Physiographic Feature: Mid-Atlantic Ridge]  [Field Program/Cruise: ODEMAR]  [Platform Name: Pourquoi Pas]</t>
+  </si>
+  <si>
+    <t>core section</t>
+  </si>
+  <si>
+    <t>[Sample Name: BARB3-615.28]  [Sample Type: Core]  [Material: Rock]  [Classification: Sedimentary]  [Field Name: Chert]  [Description: B/W chert]  [Collection Method: Coring]  [Size: 0.21 m]  [Geological Age: Paleoarchaean]  [Geological Unit: Kromberg Formation]  [Locality: Buck Reef Chert, BARB3]  [Locality Description: Barberton Greenstone Belt]  [Country: South Africa]  [City: Granville Grove 720JT]  [Current Archive: University of Johannesburg (UJ)]  [Depth in Core (min): 615.07 m]  [Depth in Core (max): 615.28 m]</t>
+  </si>
+  <si>
+    <t>borehole cuttings</t>
+  </si>
+  <si>
+    <t>[Sample Name: 50223200260000 Alcor1]  [Other Name(s): 2610-2640 ft MD]  [Sample Type: Cuttings]  [Material: Rock]  [Classification: Sedimentary]  [Description: Dry Cuttings, Box 1 of 8]  [Collection Method: Coring]  [Geological Age: Brookian]  [Geological Unit: Mikkelson Tongue of Canning Formation]  [Purpose: Dry Cuttings]  [Elevation Start: 57 meters]  [State/Province: AK]  [Depth (min): 2610 MD Feet]  [Depth (max): 2640 MD Feet]</t>
+  </si>
+  <si>
+    <t>[Sample Name: CS-4: 80-90]  [Sample Type: Cuttings]  [Material: Rock]  [Field Name: basalt, sand]  [Collection Method: Shaker table]  [Collection Method Description: Cutting sample collected from drill rig shaker table]  [Geological Age: Plio-Quaternary]  [Comment: Thermal-gradient borehole]  [Elevation Start: 1404 meters]  [Physiographic Feature: Basin &amp; Range desert basin]  [Name Of Physiographic Feature: Sevier Desert]  [Location Description: Crater Bench]  [Locality: TG Well CS-4]  [Country: United States]  [State/Province: Utah]  [Platform Type: truck-mounted drill rig]</t>
+  </si>
+  <si>
+    <t>cuttings</t>
+  </si>
+  <si>
+    <t>rock powder</t>
+  </si>
+  <si>
+    <t>[Sample Name: MB1601.373.9-p&lt;2.85]  [Sample Type: Individual Sample&gt;Powder]  [Parent IGSN: BSU0004EX]  [Material: Rock]  [Classification: Igneous]  [Collection Method: mineral separation processing]  [Collection Method Description: Parent sample crushed, density separated, this is light fraction]</t>
+  </si>
+  <si>
+    <t>XRF bead</t>
+  </si>
+  <si>
+    <t>[Sample Name: GCPUD1355]  [Other Name(s): waypoint 120, 24IX12_3]  [Sample Type: Individual Sample&gt;Bead]  [Material: Rock]  [Classification: Igneous&gt;Volcanic&gt;Mafic]  [Field Name: basalt, CRB]  [Description: "less phyric Frenchman Springs"]  [Age (min): 15.9]  [Age (max): 16]  [Collection Method: XRF bead processing]  [Collection Method Description: parent sample split, crushed, binder added, pressed into bead for analysis]  [Geological Age: Miocene]  [Geological Unit: Frenchman Springs Member of Wanapum Formation of Columbia River Basalt Group]  [Comment: composition consistent with Ginkgo; parent sample not registered]  [Purpose: XRF]  [Physiographic Feature: draw into west fork off Sheep Canyon]  [Name Of Physiographic Feature: Beezley Hills]  [Location Description: poor exposure along E Rd NW]  [Locality Description: Little Soap Lake quad]  [Country: United States]  [State/Province: Washington]</t>
+  </si>
+  <si>
+    <t>[Sample Name: Lyn 08]  [Sample Type: Individual Sample&gt;Thin Section]  [Parent IGSN: BWH00002I]  [Material: Rock]  [Classification: Ore&gt;Sulfide]  [Field Name: Ore deposit]  [Collection Method: polished thin section preparation]  [Collection Method Description: Thin section billet trimmed from slab normal to core axis in parent sample]  [Purpose: Exploratory]  [Physiographic Feature: Metamorphic terrane]  [Name Of Physiographic Feature: Pembine-Wausau Terrane]  [Locality: Lynne Deposit]  [Country: United States]  [State/Province: Wisconsin]  [County: Oneida]  [City: Tripoli]  [Field Program/Cruise: Noranda Minerals]</t>
+  </si>
+  <si>
+    <t>[Sample Name: E151]  [Sample Type: Individual Sample&gt;Specimen]  [Material: Mineral]  [Field Name: Diamond]  [Locality: Ekati Mine]  [Country: Canada]</t>
+  </si>
+  <si>
+    <t>Diamond</t>
+  </si>
+  <si>
+    <t>Calcite</t>
+  </si>
+  <si>
+    <t>[Sample Name: USFS-11290-002]  [Sample Type: Individual Sample&gt;Specimen]  [Material: Mineral]  [Classification: Calcite]  [Field Name: Calcite Cave Spar]  [Geological Age: 35.69]  [Elevation Start: 2035 meters]  [Physiographic Feature: Cave]  [Country: United States]  [State/Province: NM]</t>
+  </si>
+  <si>
+    <t>[Sample Name: Sari15-04-24]  [Sample Type: Individual Sample&gt;Specimen]  [Parent IGSN: KAK000006]  [Material: Glass]  [Field Name: Melt inclusion]  [Collection Method: inspection of thin section]  [Collection Method Description: melt inclusions identified in parent thin section]  [Size: .07 mm]  [Purpose: Targeted for microanalysis]  [Physiographic Feature: Volcano]  [Name Of Physiographic Feature: Sarigan]  [Locality: Mariana Arc]  [Country: Northern Mariana Islands]  [Field Program/Cruise: 2004 MARGINS]  [Parents: KAK000006 SARI-15-04]  [Siblings: {MNB000001 Sari15-04-01, MNB000002 Sari15-04-03, MNB000003 Sari15-04-04, MNB000004 Sari15-04-07}]</t>
+  </si>
+  <si>
+    <t>zircon grain</t>
+  </si>
+  <si>
+    <t>[Sample Name: Kn 180-2- 27-72-2]  [Sample Type: Individual Sample]  [Parent IGSN: CHE00000Z]  [Material: Mineral]  [Classification: Zircon]  [Field Name: zircon]  [Description: zircon grain]  [Collection Method: mineral grains identified in polished thin section (parent sample) for U-Pb analysis]  [Size: .27 mm]  [Name Of Physiographic Feature: Mid Atlantic Ridge]  [Parents: CHE00000Z Kn 180-2- 27-72]  [Siblings: {CHE0000F0 Kn 180-2- 27-72-1, CHE0000F2 Kn 180-2- 27-72-3, CHE0000F3 Kn 180-2- 27-72-4, CHE0000F4 Kn 180-2- 27-72-5}]</t>
+  </si>
+  <si>
+    <t>biogenic mat</t>
+  </si>
+  <si>
+    <t>[Sample Name: J797-BM1-D6-14]  [Sample Type: Individual Sample]  [Material: Biology]  [Description: Cassette D Syringe 6. Sampling site: Smaller than previous clump of fluffy yellow iron mat in shimmering water near last site. Jason T=27C. Sensor readings for area: pH=3.15v; O2=1.51ml/L.]  [Collection Method: Sampler:Biology:Syringe]  [Collection Method Description: BioMat Cassette Syringe sampler]  [Name Of Physiographic Feature: Mariana:Snail]  [Location Description: Mkr 108 site]  [Field Program/Cruise: RR1413]  [Launch Type: ROV]  [Launch Platform Name: Jason II]</t>
+  </si>
+  <si>
+    <t>Sycamore</t>
+  </si>
+  <si>
+    <t>[Sample Name: FISH-31]  [Other Name(s): 1794]  [Material: Biology]  [Field Name: Plant]  [Description: plant. collected june 2005, Sycamore, New Harbour group, unwashed]  [Purpose: The distribution and uptake of isotopes into the biosphere]  [Country: United Kingdom]</t>
+  </si>
+  <si>
+    <t>Mussel</t>
+  </si>
+  <si>
+    <t>[Sample Name: 3989]  [Sample Type: Individual Sample]  [Material: Biology]  [Collection Method: Sampler:Biology:Net]  [Comment: Mussel]  [Physiographic Feature: Vent]  [Name Of Physiographic Feature: EPR:9N:BM141]  [Field Program/Cruise: AT11-09]  [Platform Type: Ship]  [Platform Name: Atlantis]  [Launch Type: HOV]  [Launch Platform Name: Alvin]</t>
+  </si>
+  <si>
+    <t>macrofossils</t>
+  </si>
+  <si>
+    <t>[Sample Name: Bybell-006141]  [Sample Type: Individual Sample]  [Material: Biology]  [Field Name: Macrofossils]  [Geological Age: Paleocene]  [Geological Unit: Aquia]  [Locality: Glymont, Potomac River]  [Locality Description: Not Provided]  [Country: United States]  [State/Province: Maryland]</t>
+  </si>
+  <si>
+    <t>ocean trawl</t>
+  </si>
+  <si>
+    <t>[Sample Name: Otter Trawl AA CRS 953]  [Sample Type: Trawl]  [Material: Biology]  [Collection Method: Trawling&gt;OtterTrawl]  [Purpose: Species identification]  [Elevation Start: -569 meters]  [Physiographic Feature: Continental shelf]  [Name Of Physiographic Feature: West Antarctic Peninsula, Southern Ocean]</t>
+  </si>
+  <si>
+    <t>Tree disk</t>
+  </si>
+  <si>
+    <t>[Sample Name: LL1205]  [Sample Type: Other]  [Material: Biology]  [Field Name: tree disk]  [Collection Method: Chain-saw]  [Collection Method Description: Collected from dead tree]  [Comment: Field Program: PdT14]  [Physiographic Feature: Plateau]  [Name Of Physiographic Feature: Tamarugal]</t>
+  </si>
+  <si>
+    <t>mussel shell</t>
+  </si>
+  <si>
+    <t>[Sample Name: H3R]  [Sample Type: Other]  [Material: Biology]  [Classification: Macrobiology]  [Description: mussel shell]  [Age (min): 100 years]  [Age (max): 120 years]  [Collection Method Description: walk the river bank, pick up shells]  [Size: 10 cm]  [Geological Age: Holocene]  [Geological Unit: surface]  [Comment: right valve of mussels shell]  [Locality: Munson Shoals / Mussel Shoals]  [Locality Description: Bend in the Brazos River, Texas]  [Country: United States]  [State/Province: Texas]</t>
+  </si>
+  <si>
+    <t>coral</t>
+  </si>
+  <si>
+    <t>[Sample Name: L1-108]  [Sample Type: Other]  [Material: Biology]  [Classification: Macrobiology&gt;Coral]  [Field Name: Stylasteridae, Errina]  [Collection Method: Dredging; Manual]  [Collection Method Description: Coral was hand-drilled along skeleton]  [Purpose: Radiocarbon analysis]  [Elevation Start: -669 meters]  [Physiographic Feature: Upper continental slope]  [Name Of Physiographic Feature: Mertz Sill]  [Locality: Eastern Wilkes Land, Antarctica]</t>
+  </si>
+  <si>
+    <t>pulverized leaves</t>
+  </si>
+  <si>
+    <t>[Sample Name: ACSA 2059 6/9/11 Ground]  [Sample Type: Other]  [Parent IGSN: SSH000168]  [Material: Biology]  [Classification: Macrobiology]  [Field Name: Acer saccharum]  [Description: Upper Canopy Leaves (Dried and Ground)]  [Collection Method: Manual]  [Collection Method Description: Hand sampled after tree climbing, crushed split from parent sample]  [Physiographic Feature: Watershed]  [Name Of Physiographic Feature: Shale Hills Catchment]  [Country: United States]  [State/Province: Pennsylvania]</t>
+  </si>
+  <si>
+    <t>loss on ignition ash</t>
+  </si>
+  <si>
+    <t>[Sample Name: ANT14 LIT-4 D1 B2 L]  [Other Name(s): Drive 1, Bot 2-3cm]  [Sample Type: Individual Sample&gt;Powder]  [Parent IGSN: IELUJS015]  [Material: Biology]  [Classification: Macrobiology]  [Field Name: Peat]  [Description: Loss on ignition ash]  [Collection Method: Coring]  [Collection Method Description: Box Corer]  [Geological Age: Holocene]  [Comment: Sampled from parent section 9/2/14]  [Purpose: Loss On Ignition Analysis]  [Physiographic Feature: Island]  [Name Of Physiographic Feature: Litchfield Island]  [Location Description: North-facing peat bank]  [Locality: Palmer Station]  [Locality Description: 1.5km West of Palmer Station]  [Country: Antarctica]</t>
+  </si>
+  <si>
+    <t>peat core section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Sample Name: ANT14 LIT-4 D1 B2]  [Sample Type: Core Section]  [Parent IGSN: IELUJD001]  [Material: Biology]  [Classification: Macrobiology]  [Field Name: Peat]  [Description: Moss peat core sample interval]  [Collection Method: Coring]  [Collection Method Description: Box Corer]  [Size: 0.9 cm]  [Geological Age: Holocene]  [Purpose: Paleoclimatology]  [Physiographic Feature: Island]  [Name Of Physiographic Feature: Litchfield Island]  [Location Description: North-facing peat bank]  [Locality: Palmer Station]  [Locality Description: 1.5km West of Palmer Station]  [Country: Antarctica] </t>
+  </si>
+  <si>
+    <t>[Sample Name: PREH150607-1A]  [Sample Type: Individual Sample]  [Material: Soil]  [Classification: Not Provided]  [Field Name: RB-BKR-11-5 IC-BKR-11-5 brown soil pH 4.3 Depth range 0-10 cm]  [Purpose: 10Be - local erosion rate]  [Physiographic Feature: Watershed]  [Name Of Physiographic Feature: Rio Blanco]  [Locality: El Yunque National Forest]  [Locality Description: ridge left side of Rio Blanco near outlet]  [Country: Puerto Rico]</t>
+  </si>
+  <si>
+    <t>soil core section</t>
+  </si>
+  <si>
+    <t>[Sample Name: BWE201406032C1020]  [Sample Type: Core Section]  [Parent IGSN: IEBWE0003]  [Material: Soil]  [Description: Day 223 core section from unheated control plot 2C of a deep soil warming experiment]  [Collection Method: Coring&gt;HandHeldCorer]  [Collection Method Description: Collected with a multi-stage corer 5 cm in diameter using a 10 kg hand-held slide-hammer]  [Purpose: Biogeochemistry, geochemistry and microbiology]  [Physiographic Feature: Mountain]  [Name Of Physiographic Feature: Sierra Nevada foothills]  [Location Description: Mixed conifer forest]  [Locality: Blodgett Forest Research Station, University of California]  [Depth in Core (min): 10 Centimeters Below Surface]  [Depth in Core (max): 20 Centimeters Below Surface]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Provenience (Recorded): SC 8-12]   [Level: 90-130]   [WT (0.01 gram increments): 2.96]   [Max Size (5mm increments, maximum surficial length): 40.0]   [Date C14: 8020±280 BP]     [Class: Mammalia]   [Size 1: Medium]   [Order: Carnivora]   [Size 2: Medium]   [Family: Canidae]   [Size 3: Small]   [Genus: Lycalopex]   [Element: Humerus,  Distal &amp; Shaft]   [Comments: much bigger specimen than preceding] </t>
+  </si>
+  <si>
+    <t>[Sex:   Female]  [Class:   Aves]  [Order:   Galliformes]  [Family:   Phasianidae]  [Genus:   Coturnix]  [Species:   Coturnix]  [Subspecies:   japonica]  [Common Name:   Japanese quail]  [Continent/Ocean:   North America]  [Country:   USA]  [State/Province:   MA]  [Kind:   Complete skeleton]  [Received from:   Concord Field Station]  [Bio. Remarks:   wing chord 110, bill 11; had 3 eggs; found dead in pen]  [Site Name:   Bird Farm]  [Location:   Berlin]  [Specimen Remarks:   Complete skeleton]</t>
+  </si>
+  <si>
+    <t>[Laetoli Loc 8. ]  [between tuffs 5 &amp; 7]  [seed] [Pliocene]  [Plantae]</t>
+  </si>
+  <si>
+    <t>[Loc. 16]  [Laetolil Beds, Upper Unit, top part of T8]  [leaf, dicot.] [Upper Pliocene] [Plantae]</t>
+  </si>
+  <si>
+    <t>[Oleisusu]  [Laetolil Beds, ?Lower Unit]  [wood] [Pliocene]  [Plantae]</t>
+  </si>
+  <si>
+    <t>necklace fragment</t>
+  </si>
+  <si>
+    <t>[Sample Name: VC-18-03]  [Sample Type: Individual Sample&gt;Specimen]  [Material: Rock]  [Classification: Sedimentary&gt;Carbonate]  [Field Name: ooid grainstone]    [Collection Method: Manual&gt;Hammer]    [Locality: Vermillion Creek Section, Sand Wash Basin, Green River Formation]  [Country: United States]  [State/Province: Colorado]   [Collection Start Date: 2018-06-06T04:00:00Z]   [Depth (min): 0.95 meters from base of section]  [Parent: IEEJT0050 GRF-VC]</t>
   </si>
 </sst>
 </file>
@@ -2901,7 +3084,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2936,13 +3119,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2998,6 +3190,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5127,7 +5322,7 @@
         <v>382</v>
       </c>
       <c r="G52" s="19" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="100.5" x14ac:dyDescent="0.25">
@@ -5164,7 +5359,7 @@
         <v>382</v>
       </c>
       <c r="G54" s="19" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -5503,7 +5698,7 @@
         <v>382</v>
       </c>
       <c r="G67" s="19" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>614</v>
@@ -5632,7 +5827,7 @@
         <v>382</v>
       </c>
       <c r="G72" s="19" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -5672,7 +5867,7 @@
         <v>382</v>
       </c>
       <c r="G74" s="19" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>614</v>
@@ -5683,7 +5878,7 @@
         <v>382</v>
       </c>
       <c r="G75" s="19" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>614</v>
@@ -5694,7 +5889,7 @@
         <v>382</v>
       </c>
       <c r="G76" s="19" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>614</v>
@@ -5705,7 +5900,7 @@
         <v>382</v>
       </c>
       <c r="G77" s="19" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>614</v>
@@ -5987,7 +6182,7 @@
         <v>382</v>
       </c>
       <c r="G86" s="19" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>614</v>
@@ -7771,7 +7966,7 @@
         <v>382</v>
       </c>
       <c r="G141" s="19" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.25">
@@ -8634,7 +8829,7 @@
         <v>382</v>
       </c>
       <c r="G170" s="19" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="H170" s="2" t="s">
         <v>614</v>
@@ -8675,7 +8870,7 @@
         <v>382</v>
       </c>
       <c r="G172" s="19" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="H172" s="2" t="s">
         <v>614</v>
@@ -8863,7 +9058,7 @@
         <v>382</v>
       </c>
       <c r="G179" s="19" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="H179" s="2" t="s">
         <v>614</v>
@@ -8940,7 +9135,7 @@
         <v>382</v>
       </c>
       <c r="G182" s="19" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="H182" s="2" t="s">
         <v>614</v>
@@ -11814,283 +12009,548 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CA6472-78AF-47A6-B1C4-7E8E68C5F33F}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="94.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>823</v>
+      <c r="A1" s="2" t="s">
+        <v>821</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>822</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>824</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>781</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>825</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>826</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>827</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="10" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="21" t="s">
+        <v>853</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>858</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>828</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>829</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>859</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>830</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>831</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>832</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>833</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>834</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>835</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>836</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>837</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>838</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B37" s="2" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>893</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>839</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>841</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>842</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>844</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>843</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>845</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>846</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>847</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>848</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>849</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>850</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>851</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>852</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>853</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>854</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>856</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>855</v>
+      <c r="B65" s="2" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>913</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add GBIF preparations and CETAF sample types
</commit_message>
<xml_diff>
--- a/vocabulary/SampleTypeCompilation.xlsx
+++ b/vocabulary/SampleTypeCompilation.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\iSamples\metadata\vocabulary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46590782-9A26-45C8-8619-6C7D75E9B329}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB739AFE-F94E-46D3-A2A4-4960BD6028B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="360" windowWidth="16455" windowHeight="13605" firstSheet="2" activeTab="5" xr2:uid="{D08A62D1-934B-493D-9C48-9223CA83C33D}"/>
+    <workbookView xWindow="3045" yWindow="375" windowWidth="18945" windowHeight="13605" activeTab="3" xr2:uid="{D08A62D1-934B-493D-9C48-9223CA83C33D}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleTypes" sheetId="1" r:id="rId1"/>
     <sheet name="OtherTypes" sheetId="2" r:id="rId2"/>
-    <sheet name="Synthesis" sheetId="3" r:id="rId3"/>
-    <sheet name="sampledFeature" sheetId="6" r:id="rId4"/>
-    <sheet name="procedure" sheetId="7" r:id="rId5"/>
-    <sheet name="CardDescriptions" sheetId="8" r:id="rId6"/>
+    <sheet name="GBIF  oc.v_preparations summary" sheetId="9" r:id="rId3"/>
+    <sheet name="CETAF SampleTypes" sheetId="10" r:id="rId4"/>
+    <sheet name="Synthesis" sheetId="3" r:id="rId5"/>
+    <sheet name="sampledFeature" sheetId="6" r:id="rId6"/>
+    <sheet name="procedure" sheetId="7" r:id="rId7"/>
+    <sheet name="CardDescriptions" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SampleTypes!$A$1:$A$164</definedName>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2076" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2553" uniqueCount="1172">
   <si>
     <t>Identical split(s) of an original sample submitted blindly to the laboratory to test reproducibility (bias) of results.  Should be related to a previous original specimen.</t>
   </si>
@@ -2981,12 +2983,765 @@
   <si>
     <t>[Sample Name: VC-18-03]  [Sample Type: Individual Sample&gt;Specimen]  [Material: Rock]  [Classification: Sedimentary&gt;Carbonate]  [Field Name: ooid grainstone]    [Collection Method: Manual&gt;Hammer]    [Locality: Vermillion Creek Section, Sand Wash Basin, Green River Formation]  [Country: United States]  [State/Province: Colorado]   [Collection Start Date: 2018-06-06T04:00:00Z]   [Depth (min): 0.95 meters from base of section]  [Parent: IEEJT0050 GRF-VC]</t>
   </si>
+  <si>
+    <t>wet</t>
+  </si>
+  <si>
+    <t>slice</t>
+  </si>
+  <si>
+    <t>skeletonized??</t>
+  </si>
+  <si>
+    <t>SEM, alcohol</t>
+  </si>
+  <si>
+    <t>SEM</t>
+  </si>
+  <si>
+    <t>residue pellet</t>
+  </si>
+  <si>
+    <t>preserved</t>
+  </si>
+  <si>
+    <t>polish</t>
+  </si>
+  <si>
+    <t>planting</t>
+  </si>
+  <si>
+    <t>pin, microvial</t>
+  </si>
+  <si>
+    <t>pin</t>
+  </si>
+  <si>
+    <t>on plinth</t>
+  </si>
+  <si>
+    <t>not specified</t>
+  </si>
+  <si>
+    <t>mummification</t>
+  </si>
+  <si>
+    <t>mounted on slide,alcohol</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>6.0.0</t>
+  </si>
+  <si>
+    <t>mounted on slide, SEM</t>
+  </si>
+  <si>
+    <t>5.1.1</t>
+  </si>
+  <si>
+    <t>mounted on slide, PVL</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>5.0.0</t>
+  </si>
+  <si>
+    <t>mounted on slide, glycerol</t>
+  </si>
+  <si>
+    <t>drug</t>
+  </si>
+  <si>
+    <t>4.0.0</t>
+  </si>
+  <si>
+    <t>mounted on slide</t>
+  </si>
+  <si>
+    <t>slide</t>
+  </si>
+  <si>
+    <t>3.0.0</t>
+  </si>
+  <si>
+    <t>mounted</t>
+  </si>
+  <si>
+    <t>cast</t>
+  </si>
+  <si>
+    <t>3.1.0</t>
+  </si>
+  <si>
+    <t>molding</t>
+  </si>
+  <si>
+    <t>bird nest, egg</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>liquid preservation</t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t>2.1.0</t>
+  </si>
+  <si>
+    <t>herbarium sheet</t>
+  </si>
+  <si>
+    <t>bird nest</t>
+  </si>
+  <si>
+    <t>2.0.0</t>
+  </si>
+  <si>
+    <t>freeze, dried</t>
+  </si>
+  <si>
+    <t>tissue</t>
+  </si>
+  <si>
+    <t>1.5.0</t>
+  </si>
+  <si>
+    <t>freeze</t>
+  </si>
+  <si>
+    <t>human remains</t>
+  </si>
+  <si>
+    <t>1.4.0</t>
+  </si>
+  <si>
+    <t>formalin</t>
+  </si>
+  <si>
+    <t>DNA</t>
+  </si>
+  <si>
+    <t>1.3.0</t>
+  </si>
+  <si>
+    <t>fixation</t>
+  </si>
+  <si>
+    <t>Tree part</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t>elution buffer</t>
+  </si>
+  <si>
+    <t>1.2.2</t>
+  </si>
+  <si>
+    <t>dry mounted</t>
+  </si>
+  <si>
+    <t>plant part</t>
+  </si>
+  <si>
+    <t>1.2.1</t>
+  </si>
+  <si>
+    <t>dried, SEM</t>
+  </si>
+  <si>
+    <t>plant</t>
+  </si>
+  <si>
+    <t>1.2.0</t>
+  </si>
+  <si>
+    <t>dried, alcohol, SEM</t>
+  </si>
+  <si>
+    <t>bird</t>
+  </si>
+  <si>
+    <t>1.1.3</t>
+  </si>
+  <si>
+    <t>dried</t>
+  </si>
+  <si>
+    <t>bone</t>
+  </si>
+  <si>
+    <t>1.1.2.1</t>
+  </si>
+  <si>
+    <t>C&amp;S without KOH</t>
+  </si>
+  <si>
+    <t>Bird part</t>
+  </si>
+  <si>
+    <t>1.1.2.3</t>
+  </si>
+  <si>
+    <t>Brightened and colored</t>
+  </si>
+  <si>
+    <t>tooth</t>
+  </si>
+  <si>
+    <t>1.1.2.2</t>
+  </si>
+  <si>
+    <t>alcohol, SEM</t>
+  </si>
+  <si>
+    <t>animal part</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>alcohol, freeze</t>
+  </si>
+  <si>
+    <t>whole animal</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>alcohol, dried</t>
+  </si>
+  <si>
+    <t>animal</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
+    <t>alcohol</t>
+  </si>
+  <si>
+    <t>biological specimen</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>acid treatment</t>
+  </si>
+  <si>
+    <t>0.0.0</t>
+  </si>
+  <si>
+    <t>sample type</t>
+  </si>
+  <si>
+    <t>preservationMethod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtain from </t>
+  </si>
+  <si>
+    <t>https://github.com/tdwg/mids/issues/14#issuecomment-763578403</t>
+  </si>
+  <si>
+    <t>GBIF data in gbif_export_20200611_v2</t>
+  </si>
+  <si>
+    <t>SEM preparation</t>
+  </si>
+  <si>
+    <t>https://www.gu.se/en/core-facilities/sem-sample-preparation-techniques</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>sort</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>basisOfRecord</t>
+  </si>
+  <si>
+    <t>preparations</t>
+  </si>
+  <si>
+    <t>sampled feature</t>
+  </si>
+  <si>
+    <t>specimenType</t>
+  </si>
+  <si>
+    <t>https://github.com/tdwg/mids/issues/5</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Occurrence</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1qUMeCcC2VsF487PMNODE1bA3VsCTZH2ydNQ0_LWLnbU/edit#gid=234199043</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>PhysicalObject</t>
+  </si>
+  <si>
+    <t>FossilSpecimen</t>
+  </si>
+  <si>
+    <t>coal ball</t>
+  </si>
+  <si>
+    <t>rock</t>
+  </si>
+  <si>
+    <t>CETAF Digitization Working Group, 7th December 2020</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>Macrofissil</t>
+  </si>
+  <si>
+    <t>https://cetafdigitization.biowikifarm.net/cdig/</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>LivingSpecimen</t>
+  </si>
+  <si>
+    <t>cytological specimen</t>
+  </si>
+  <si>
+    <t>animal or plant cell</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>living</t>
+  </si>
+  <si>
+    <t>living organism</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>MaterialSample</t>
+  </si>
+  <si>
+    <t>bark</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Beak</t>
+  </si>
+  <si>
+    <t>Bird</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Cast</t>
+  </si>
+  <si>
+    <t>whatever made the mold for the casting</t>
+  </si>
+  <si>
+    <t>guessing this means a cast of something was made in the field</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>Claw</t>
+  </si>
+  <si>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>core sample</t>
+  </si>
+  <si>
+    <t>what was cored? A tree, or the earth?</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>DNA sample</t>
+  </si>
+  <si>
+    <t>biologic specimen</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>ethnobotanical object</t>
+  </si>
+  <si>
+    <t>don't know if this is whole or part</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>Feather</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>frozen tissue</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>fruit/cone</t>
+  </si>
+  <si>
+    <t>FU</t>
+  </si>
+  <si>
+    <t>Fur or hair</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>Microscope slide</t>
+  </si>
+  <si>
+    <t>microscope slide</t>
+  </si>
+  <si>
+    <t>whats on the slide?</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>Peel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peel </t>
+  </si>
+  <si>
+    <t>need detail on what this is</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Pharmaceutical</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>Pollen</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>SEM stub</t>
+  </si>
+  <si>
+    <t>whats on the stub?</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>what is the material for shell, bone, etc? not really organic</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>Skeleton</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>Skin</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>Spore</t>
+  </si>
+  <si>
+    <t>fungus</t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>Tooth</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>EG</t>
+  </si>
+  <si>
+    <t>PreservedSpecimen</t>
+  </si>
+  <si>
+    <t>Egg</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>HerbariumSheet</t>
+  </si>
+  <si>
+    <t>HW</t>
+  </si>
+  <si>
+    <t>HerbariumSheet:dormant</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>HerbariumSheet:flower</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>HerbariumSheet:fruit</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>HerbariumSheet:seedling</t>
+  </si>
+  <si>
+    <t>HV</t>
+  </si>
+  <si>
+    <t>HerbariumSheet:vegetative</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>LiquidPreserved</t>
+  </si>
+  <si>
+    <t>container with liquid</t>
+  </si>
+  <si>
+    <t>assume preserved item is some kind of organism</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>LiquidPreserved:alcohol</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>LiquidPreserved:formalin</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>LiquidPreserved:glycerin</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>Pinned</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>Silica gel</t>
+  </si>
+  <si>
+    <t>whole or part?</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>Stuffed</t>
+  </si>
+  <si>
+    <t>UD</t>
+  </si>
+  <si>
+    <t>Unmounted dried specimen</t>
+  </si>
+  <si>
+    <t>Related resources</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t>StillImage</t>
+  </si>
+  <si>
+    <t>HumanObservation</t>
+  </si>
+  <si>
+    <t>drawing in b&amp;w</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>drawing in color</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>drawing made with aid of microscope</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Painting</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>Spore print</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>MachineObservation</t>
+  </si>
+  <si>
+    <t>Photograph</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t>Photograph:b&amp;w</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Photograph:color</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>Photograph:lightMicroscope</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>Photograph:slide</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>Scan</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>SEM micrograph</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>Transmission electron micrograph</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3069,6 +3824,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3129,12 +3945,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3195,11 +4015,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="6" xr:uid="{AA359D7C-8588-48E7-BA79-2FB9E1F0F3C9}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{1E5144E3-89D2-4FFB-A691-11424BD1BBF2}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{A51B88D9-E0D5-4AE8-B7F7-35E1FFE7F975}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -9430,6 +10300,2048 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3C2B4E-2650-4C5F-8296-B9D8AAB75C6B}">
+  <dimension ref="A1:L41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" style="22" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="22"/>
+    <col min="6" max="6" width="16.85546875" style="22" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
+        <v>1015</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>1007</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" s="22">
+        <v>18384</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>1006</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="G2" s="22">
+        <v>1663</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>1009</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B3" s="22">
+        <v>74</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G3" s="22">
+        <v>8947</v>
+      </c>
+      <c r="K3" s="26" t="s">
+        <v>1011</v>
+      </c>
+      <c r="L3"/>
+    </row>
+    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B4" s="22">
+        <v>11058</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>1000</v>
+      </c>
+      <c r="G4" s="22">
+        <v>12</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>1012</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>999</v>
+      </c>
+      <c r="B5" s="22">
+        <v>7</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>998</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>997</v>
+      </c>
+      <c r="G5" s="22">
+        <v>2742</v>
+      </c>
+      <c r="K5"/>
+      <c r="L5"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>996</v>
+      </c>
+      <c r="B6" s="22">
+        <v>2</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>995</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>994</v>
+      </c>
+      <c r="G6" s="22">
+        <v>58776</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
+        <v>993</v>
+      </c>
+      <c r="B7" s="22">
+        <v>18</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>992</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>991</v>
+      </c>
+      <c r="G7" s="22">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
+        <v>990</v>
+      </c>
+      <c r="B8" s="22">
+        <v>196</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>989</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>988</v>
+      </c>
+      <c r="G8" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>987</v>
+      </c>
+      <c r="B9" s="22">
+        <v>3</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>986</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>985</v>
+      </c>
+      <c r="G9" s="22">
+        <v>86835</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>984</v>
+      </c>
+      <c r="B10" s="22">
+        <v>10596</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>983</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>982</v>
+      </c>
+      <c r="G10" s="22">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
+        <v>981</v>
+      </c>
+      <c r="B11" s="22">
+        <v>1</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>980</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>979</v>
+      </c>
+      <c r="G11" s="22">
+        <v>1011812</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>978</v>
+      </c>
+      <c r="B12" s="22">
+        <v>1</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>977</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>976</v>
+      </c>
+      <c r="G12" s="22">
+        <v>3310</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
+        <v>975</v>
+      </c>
+      <c r="B13" s="22">
+        <v>9</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>974</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>477</v>
+      </c>
+      <c r="G13" s="22">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>973</v>
+      </c>
+      <c r="B14" s="22">
+        <v>42</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>972</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>971</v>
+      </c>
+      <c r="G14" s="22">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
+        <v>970</v>
+      </c>
+      <c r="B15" s="22">
+        <v>5</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>969</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>968</v>
+      </c>
+      <c r="G15" s="22">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
+        <v>967</v>
+      </c>
+      <c r="B16" s="22">
+        <v>6</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>966</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>965</v>
+      </c>
+      <c r="G16" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="22" t="s">
+        <v>964</v>
+      </c>
+      <c r="B17" s="22">
+        <v>581</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>963</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>962</v>
+      </c>
+      <c r="G17" s="22">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
+        <v>961</v>
+      </c>
+      <c r="B18" s="22">
+        <v>8</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>960</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>959</v>
+      </c>
+      <c r="G18" s="22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="s">
+        <v>958</v>
+      </c>
+      <c r="B19" s="22">
+        <v>164</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>956</v>
+      </c>
+      <c r="G19" s="22">
+        <v>11473</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
+        <v>955</v>
+      </c>
+      <c r="B20" s="22">
+        <v>6855</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>954</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>953</v>
+      </c>
+      <c r="G20" s="22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="22" t="s">
+        <v>952</v>
+      </c>
+      <c r="B21" s="22">
+        <v>12</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>951</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>950</v>
+      </c>
+      <c r="G21" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="22" t="s">
+        <v>949</v>
+      </c>
+      <c r="B22" s="22">
+        <v>4427</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>948</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>947</v>
+      </c>
+      <c r="G22" s="22">
+        <v>6647</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="22" t="s">
+        <v>946</v>
+      </c>
+      <c r="B23" s="22">
+        <v>6446</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>945</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>944</v>
+      </c>
+      <c r="G23" s="22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="22" t="s">
+        <v>943</v>
+      </c>
+      <c r="B24" s="22">
+        <v>151</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>942</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>941</v>
+      </c>
+      <c r="G24" s="22">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="22" t="s">
+        <v>940</v>
+      </c>
+      <c r="B25" s="22">
+        <v>42</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>939</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="G25" s="22">
+        <v>5954513</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="22" t="s">
+        <v>938</v>
+      </c>
+      <c r="B26" s="22">
+        <v>4</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>937</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>936</v>
+      </c>
+      <c r="G26" s="22">
+        <v>4588</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="22" t="s">
+        <v>935</v>
+      </c>
+      <c r="B27" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="22" t="s">
+        <v>934</v>
+      </c>
+      <c r="B28" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="22" t="s">
+        <v>933</v>
+      </c>
+      <c r="B29" s="22">
+        <v>29115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>932</v>
+      </c>
+      <c r="B30" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="22" t="s">
+        <v>931</v>
+      </c>
+      <c r="B31" s="22">
+        <v>322683</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="22" t="s">
+        <v>930</v>
+      </c>
+      <c r="B32" s="22">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="22" t="s">
+        <v>929</v>
+      </c>
+      <c r="B33" s="22">
+        <v>26041</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="22" t="s">
+        <v>928</v>
+      </c>
+      <c r="B34" s="22">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="22" t="s">
+        <v>927</v>
+      </c>
+      <c r="B35" s="22">
+        <v>16660</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="22" t="s">
+        <v>926</v>
+      </c>
+      <c r="B36" s="22">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="22" t="s">
+        <v>925</v>
+      </c>
+      <c r="B37" s="22">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="22" t="s">
+        <v>924</v>
+      </c>
+      <c r="B38" s="22">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="22" t="s">
+        <v>923</v>
+      </c>
+      <c r="B39" s="22">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="22" t="s">
+        <v>922</v>
+      </c>
+      <c r="B40" s="22">
+        <v>2656</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="22" t="s">
+        <v>921</v>
+      </c>
+      <c r="B41" s="22">
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" location="issuecomment-763578403" xr:uid="{8F8F5FCB-1821-489F-A6F2-4589D3D11E42}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251F4142-FF2C-45DC-9BB3-06F399484576}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:J62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="24" style="31" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="31" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" style="31" customWidth="1"/>
+    <col min="5" max="5" width="20" style="31" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="31"/>
+    <col min="7" max="7" width="30.7109375" style="31" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" style="31" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="31"/>
+    <col min="10" max="10" width="26" style="31" customWidth="1"/>
+    <col min="11" max="16384" width="14.42578125" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>1021</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="34" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E3" s="33"/>
+      <c r="F3" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>1032</v>
+      </c>
+      <c r="H3" s="35"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="36" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E4" s="33"/>
+      <c r="F4" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>1032</v>
+      </c>
+      <c r="H4" s="35"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="34" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>526</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+    </row>
+    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>1043</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>526</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+    </row>
+    <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+    </row>
+    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>1050</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+    </row>
+    <row r="9" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F9" s="33"/>
+      <c r="G9" s="38" t="s">
+        <v>1054</v>
+      </c>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+    </row>
+    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>1057</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+    </row>
+    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E11" s="33"/>
+      <c r="F11" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="G11" s="33"/>
+      <c r="H11" s="35" t="s">
+        <v>1060</v>
+      </c>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+    </row>
+    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>528</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+    </row>
+    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>526</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+    </row>
+    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="32" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+    </row>
+    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="32" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>962</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+    </row>
+    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="32" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+    </row>
+    <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="32" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+    </row>
+    <row r="18" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="32" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E18" s="33"/>
+      <c r="F18" s="35" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G18" s="33"/>
+      <c r="H18" s="35" t="s">
+        <v>1078</v>
+      </c>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+    </row>
+    <row r="19" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="32" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E19" s="33"/>
+      <c r="F19" s="35" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G19" s="33"/>
+      <c r="H19" s="35" t="s">
+        <v>1082</v>
+      </c>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+    </row>
+    <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="32" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E20" s="33"/>
+      <c r="F20" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="G20" s="33"/>
+      <c r="H20" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+    </row>
+    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="32" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+    </row>
+    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="32" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>1089</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+    </row>
+    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="32" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G23" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+    </row>
+    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="32" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E24" s="33"/>
+      <c r="F24" s="35" t="s">
+        <v>1092</v>
+      </c>
+      <c r="G24" s="33"/>
+      <c r="H24" s="35" t="s">
+        <v>1093</v>
+      </c>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+    </row>
+    <row r="25" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="32" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>327</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G25" s="39" t="s">
+        <v>257</v>
+      </c>
+      <c r="H25" s="33" t="s">
+        <v>1095</v>
+      </c>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+    </row>
+    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="32" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G26" s="39" t="s">
+        <v>257</v>
+      </c>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+    </row>
+    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="32" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G27" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+    </row>
+    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="32" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G28" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+    </row>
+    <row r="29" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="32" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G29" s="39" t="s">
+        <v>257</v>
+      </c>
+      <c r="H29" s="33" t="s">
+        <v>1095</v>
+      </c>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+    </row>
+    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="32" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>366</v>
+      </c>
+      <c r="E30" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G30" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+    </row>
+    <row r="31" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="32" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D31" s="37" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F31" s="33"/>
+      <c r="G31" s="39" t="s">
+        <v>257</v>
+      </c>
+      <c r="H31" s="33" t="s">
+        <v>1095</v>
+      </c>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+    </row>
+    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="32" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>1110</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>958</v>
+      </c>
+      <c r="G32" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+    </row>
+    <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="32" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>1112</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>958</v>
+      </c>
+      <c r="G33" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+    </row>
+    <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="32" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B34" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>1114</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>958</v>
+      </c>
+      <c r="G34" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+    </row>
+    <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="32" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E35" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F35" s="35" t="s">
+        <v>958</v>
+      </c>
+      <c r="G35" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
+    </row>
+    <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="32" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C36" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>958</v>
+      </c>
+      <c r="G36" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
+    </row>
+    <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="32" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E37" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F37" s="35" t="s">
+        <v>958</v>
+      </c>
+      <c r="G37" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
+    </row>
+    <row r="38" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A38" s="32" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>1122</v>
+      </c>
+      <c r="E38" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F38" s="35" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G38" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H38" s="33" t="s">
+        <v>1124</v>
+      </c>
+      <c r="I38" s="33"/>
+      <c r="J38" s="33"/>
+    </row>
+    <row r="39" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A39" s="32" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E39" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G39" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H39" s="33" t="s">
+        <v>1124</v>
+      </c>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+    </row>
+    <row r="40" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A40" s="32" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B40" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E40" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G40" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H40" s="33" t="s">
+        <v>1124</v>
+      </c>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+    </row>
+    <row r="41" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A41" s="32" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>1130</v>
+      </c>
+      <c r="E41" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G41" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H41" s="33" t="s">
+        <v>1124</v>
+      </c>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+    </row>
+    <row r="42" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="32" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B42" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C42" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E42" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F42" s="35" t="s">
+        <v>526</v>
+      </c>
+      <c r="G42" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H42" s="33"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="33"/>
+    </row>
+    <row r="43" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="32" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B43" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C43" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D43" s="37" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E43" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F43" s="39" t="s">
+        <v>526</v>
+      </c>
+      <c r="G43" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H43" s="35" t="s">
+        <v>1135</v>
+      </c>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+    </row>
+    <row r="44" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="32" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E44" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F44" s="39" t="s">
+        <v>526</v>
+      </c>
+      <c r="G44" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H44" s="35" t="s">
+        <v>1135</v>
+      </c>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
+    </row>
+    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="32" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B45" s="32" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C45" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D45" s="32" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E45" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F45" s="39" t="s">
+        <v>526</v>
+      </c>
+      <c r="G45" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="H45" s="35" t="s">
+        <v>1135</v>
+      </c>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+    </row>
+    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="G46" s="41"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+    </row>
+    <row r="48" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="42" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+    </row>
+    <row r="49" spans="1:4" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="40" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B49" s="40" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C49" s="40" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D49" s="40" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="40" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B50" s="40" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C50" s="40" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D50" s="40" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="40" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B51" s="40" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C51" s="40" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D51" s="40" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="40" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B52" s="40" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C52" s="40" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D52" s="40" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="40" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B53" s="40" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C53" s="40" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D53" s="40" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="40" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B54" s="40" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C54" s="40" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D54" s="40" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="40" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B55" s="40" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C55" s="40" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D55" s="40" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="40" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B56" s="40" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C56" s="40" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D56" s="40" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="40" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B57" s="40" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C57" s="40" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D57" s="40" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A58" s="40" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B58" s="40" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C58" s="40" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D58" s="40" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="40" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B59" s="40" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C59" s="40" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D59" s="40" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A60" s="40" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B60" s="40" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C60" s="40" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D60" s="40" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A61" s="40" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B61" s="40" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C61" s="40" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D61" s="40" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A62" s="40" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B62" s="40" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C62" s="40" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D62" s="40" t="s">
+        <v>820</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:I4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J1" r:id="rId1" xr:uid="{A55B9E54-C501-41F9-A237-91D2116DB6F2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7462EFFD-5DEC-48C8-895D-422909D578AE}">
   <dimension ref="A1:J200"/>
   <sheetViews>
@@ -10475,7 +13387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E369966-9B61-468E-AAF8-630DA80EB960}">
   <dimension ref="A1:I43"/>
   <sheetViews>
@@ -11327,7 +14239,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D4AD3E-BF3E-4556-BE4E-E5EAD7F5CF3E}">
   <dimension ref="A1:G45"/>
   <sheetViews>
@@ -12007,11 +14919,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CA6472-78AF-47A6-B1C4-7E8E68C5F33F}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add CETAF and GBIF preparations
</commit_message>
<xml_diff>
--- a/vocabulary/SampleTypeCompilation.xlsx
+++ b/vocabulary/SampleTypeCompilation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\iSamples\metadata\vocabulary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB739AFE-F94E-46D3-A2A4-4960BD6028B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B3F45E-BA5C-4330-9E7A-031F60FE6C79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="375" windowWidth="18945" windowHeight="13605" activeTab="3" xr2:uid="{D08A62D1-934B-493D-9C48-9223CA83C33D}"/>
+    <workbookView xWindow="1620" yWindow="705" windowWidth="24780" windowHeight="13485" activeTab="3" xr2:uid="{D08A62D1-934B-493D-9C48-9223CA83C33D}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleTypes" sheetId="1" r:id="rId1"/>

</xml_diff>